<commit_message>
ElLeis - UPDATE ON DEFAULT WEBPAGE, DATERANGED WEBPAGE, MT TRACKER, SCREENSHOT, FIXED BUGS AND VULNERABILITES
</commit_message>
<xml_diff>
--- a/mt-tracker/April 2020/Elijah.Leis-TimeTrackerDocument-april.xlsx
+++ b/mt-tracker/April 2020/Elijah.Leis-TimeTrackerDocument-april.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99fdc28b3772e4a9/Documents/GitHub/MT3.5-CAM/mt-tracker/April 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Documents\GitHub\MT3.5-CAM\mt-tracker\April 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9283D8C0-B8C4-4404-8F01-B64CBFD8B3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5F944047-A19F-4DB0-9187-A8C07A157F5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98F465C-89F0-40A6-9AFB-184B8E3C6A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Resource Name:</t>
   </si>
@@ -166,6 +166,51 @@
   </si>
   <si>
     <t>researched about what API to use for the daterange picker and coded</t>
+  </si>
+  <si>
+    <t>Populated availability table</t>
+  </si>
+  <si>
+    <t>Coded the query to be use for the default website</t>
+  </si>
+  <si>
+    <t>Fixed the buged in availability table and double check each terminal</t>
+  </si>
+  <si>
+    <t>Recalculated the duration_sec column and availability_percentage</t>
+  </si>
+  <si>
+    <t>Inserted and updated the availability table</t>
+  </si>
+  <si>
+    <t>Coded the updated query to be use for the default webpage and dateranged webpage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coded the default and date range webpage with the use of the updated query </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed bugs found on the sonar scan </t>
+  </si>
+  <si>
+    <t>Rewritten the query to be use for the default webpage and dateranged webpaged</t>
+  </si>
+  <si>
+    <t>Kept coding to query to be use while thinking of chart to use for the system</t>
+  </si>
+  <si>
+    <t>Coded the line chart in the dummy webpage for testing and experimenting</t>
+  </si>
+  <si>
+    <t>Implemented line chart in the system but won't show</t>
+  </si>
+  <si>
+    <t>Updated the inventory table in the database to put ISO code. (randomly) Not all ISO code was inputted</t>
+  </si>
+  <si>
+    <t>Updated the query to show only the region code with the highest availability</t>
+  </si>
+  <si>
+    <t>Coded the default and date range webpage with the updated query</t>
   </si>
 </sst>
 </file>
@@ -425,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -457,9 +502,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -469,25 +511,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -499,8 +529,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AC57"/>
+  <dimension ref="B1:AC72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:D28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z46" sqref="Z46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -795,7 +846,7 @@
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
     <col min="4" max="4" width="42.5546875" customWidth="1"/>
     <col min="5" max="20" width="3.6640625" customWidth="1"/>
-    <col min="21" max="21" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -825,11 +876,11 @@
       </c>
     </row>
     <row r="6" spans="2:29" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10">
         <v>43922</v>
       </c>
@@ -904,118 +955,118 @@
       </c>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="15">
-        <f>SUM(E8:E40)</f>
+        <f>SUM(E8:E55)</f>
         <v>8</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" ref="F7:G7" si="0">SUM(F8:F37)</f>
+        <f>SUM(F8:F52)</f>
         <v>10</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
+        <f>SUM(G8:G52)</f>
         <v>20</v>
       </c>
       <c r="H7" s="15">
-        <f>SUM(H8:H40)</f>
+        <f>SUM(H8:H55)</f>
         <v>4</v>
       </c>
       <c r="I7" s="15">
-        <f>SUM(I8:I40)</f>
+        <f>SUM(I8:I55)</f>
         <v>4</v>
       </c>
       <c r="J7" s="15">
-        <f>SUM(J8:J37)</f>
+        <f>SUM(J8:J52)</f>
         <v>8</v>
       </c>
       <c r="K7" s="15">
-        <f t="shared" ref="K7:N7" si="1">SUM(K8:K37)</f>
+        <f>SUM(K8:K52)</f>
         <v>19</v>
       </c>
       <c r="L7" s="15">
-        <f t="shared" si="1"/>
+        <f>SUM(L8:L52)</f>
         <v>10</v>
       </c>
       <c r="M7" s="15">
-        <f t="shared" si="1"/>
+        <f>SUM(M8:M52)</f>
         <v>5</v>
       </c>
       <c r="N7" s="15">
-        <f t="shared" si="1"/>
+        <f>SUM(N8:N52)</f>
         <v>12</v>
       </c>
       <c r="O7" s="15">
-        <f>SUM(O8:O40)</f>
+        <f>SUM(O8:O55)</f>
         <v>0</v>
       </c>
       <c r="P7" s="15">
-        <f>SUM(P8:P40)</f>
+        <f>SUM(P8:P55)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="15">
-        <f>SUM(Q8:Q37)</f>
+        <f>SUM(Q8:Q52)</f>
         <v>9</v>
       </c>
       <c r="R7" s="15">
-        <f t="shared" ref="R7:T7" si="2">SUM(R8:R37)</f>
+        <f>SUM(R8:R52)</f>
         <v>9</v>
       </c>
       <c r="S7" s="15">
-        <f t="shared" si="2"/>
+        <f>SUM(S8:S52)</f>
         <v>10</v>
       </c>
       <c r="T7" s="15">
-        <f t="shared" si="2"/>
+        <f>SUM(T8:T52)</f>
         <v>13</v>
       </c>
       <c r="U7" s="15">
-        <f t="shared" ref="U7:AB7" si="3">SUM(U8:U37)</f>
-        <v>0</v>
+        <f>SUM(U8:U52)</f>
+        <v>10</v>
       </c>
       <c r="V7" s="15">
-        <f t="shared" si="3"/>
+        <f>SUM(V8:V52)</f>
         <v>0</v>
       </c>
       <c r="W7" s="15">
-        <f t="shared" si="3"/>
+        <f>SUM(W8:W52)</f>
         <v>0</v>
       </c>
       <c r="X7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(X8:X52)</f>
+        <v>12</v>
       </c>
       <c r="Y7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(Y8:Y52)</f>
+        <v>18</v>
       </c>
       <c r="Z7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(Z8:Z52)</f>
+        <v>9</v>
       </c>
       <c r="AA7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(AA8:AA52)</f>
+        <v>16</v>
       </c>
       <c r="AB7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(AB8:AB52)</f>
+        <v>5</v>
       </c>
       <c r="AC7" s="14">
         <f>SUM(E7:AB7)</f>
-        <v>141</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="12">
         <v>8</v>
       </c>
@@ -1043,16 +1094,16 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="14">
-        <f t="shared" ref="AC8:AC37" si="4">SUM(E8:T8)</f>
+        <f>SUM(E8:T8)</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12">
         <v>10</v>
@@ -1080,16 +1131,16 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
       <c r="AC9" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E9:T9)</f>
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12">
@@ -1117,16 +1168,16 @@
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E10:T10)</f>
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12">
@@ -1154,16 +1205,16 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
       <c r="AC11" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E11:T11)</f>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1191,16 +1242,16 @@
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E12:T12)</f>
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -1228,16 +1279,16 @@
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E13:T13)</f>
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1265,16 +1316,16 @@
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E14:T14)</f>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -1306,16 +1357,16 @@
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
       <c r="AC15" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E15:T15)</f>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -1343,16 +1394,16 @@
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E16:T16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -1380,16 +1431,16 @@
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E17:T17)</f>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -1417,16 +1468,16 @@
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
       <c r="AC18" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E18:T18)</f>
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -1454,16 +1505,16 @@
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E19:T19)</f>
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -1491,16 +1542,16 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
       <c r="AC20" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E20:T20)</f>
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -1528,16 +1579,16 @@
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
       <c r="AC21" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E21:T21)</f>
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1565,16 +1616,16 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E22:T22)</f>
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -1602,16 +1653,16 @@
       <c r="AA23" s="12"/>
       <c r="AB23" s="12"/>
       <c r="AC23" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E23:T23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -1639,16 +1690,16 @@
       <c r="AA24" s="12"/>
       <c r="AB24" s="12"/>
       <c r="AC24" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E24:T24)</f>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -1676,16 +1727,16 @@
       <c r="AA25" s="12"/>
       <c r="AB25" s="12"/>
       <c r="AC25" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E25:T25)</f>
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -1713,16 +1764,16 @@
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AC26" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E26:T26)</f>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -1750,16 +1801,16 @@
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
       <c r="AC27" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E27:T27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -1787,16 +1838,16 @@
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E28:T28)</f>
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -1824,16 +1875,16 @@
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
       <c r="AC29" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E29:T29)</f>
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -1861,16 +1912,16 @@
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E30:T30)</f>
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -1898,16 +1949,16 @@
       <c r="AA31" s="12"/>
       <c r="AB31" s="12"/>
       <c r="AC31" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E31:T31)</f>
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
@@ -1935,16 +1986,16 @@
       <c r="AA32" s="12"/>
       <c r="AB32" s="12"/>
       <c r="AC32" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E32:T32)</f>
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
@@ -1972,16 +2023,16 @@
       <c r="AA33" s="12"/>
       <c r="AB33" s="12"/>
       <c r="AC33" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E33:T33)</f>
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
@@ -2009,16 +2060,16 @@
       <c r="AA34" s="12"/>
       <c r="AB34" s="12"/>
       <c r="AC34" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E34:T34)</f>
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
@@ -2046,16 +2097,16 @@
       <c r="AA35" s="12"/>
       <c r="AB35" s="12"/>
       <c r="AC35" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E35:T35)</f>
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -2083,14 +2134,16 @@
       <c r="AA36" s="12"/>
       <c r="AB36" s="12"/>
       <c r="AC36" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(E36:T36)</f>
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="B37" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -2107,7 +2160,9 @@
       <c r="R37" s="12"/>
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
-      <c r="U37" s="12"/>
+      <c r="U37" s="12">
+        <v>10</v>
+      </c>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
@@ -2115,122 +2170,48 @@
       <c r="Z37" s="12"/>
       <c r="AA37" s="12"/>
       <c r="AB37" s="12"/>
-      <c r="AC37" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="AC37" s="14"/>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="15">
-        <f t="shared" ref="E38:T38" si="5">SUM(E39:E40)</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L38" s="15">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="15">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="R38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S38" s="15">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-      <c r="T38" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U38" s="15">
-        <f t="shared" ref="U38:AB38" si="6">SUM(U39:U40)</f>
-        <v>0</v>
-      </c>
-      <c r="V38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AA38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB38" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC38" s="13">
-        <f>SUM(E38:AB38)</f>
-        <v>6.5</v>
-      </c>
+      <c r="B38" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+      <c r="W38" s="12"/>
+      <c r="X38" s="12">
+        <v>8</v>
+      </c>
+      <c r="Y38" s="12"/>
+      <c r="Z38" s="12"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="12"/>
+      <c r="AC38" s="14"/>
     </row>
     <row r="39" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="28"/>
+      <c r="B39" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
@@ -2238,38 +2219,33 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="12">
-        <v>3</v>
-      </c>
+      <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
-      <c r="Q39" s="12">
-        <v>1</v>
-      </c>
+      <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
-      <c r="S39" s="12">
-        <v>2.5</v>
-      </c>
+      <c r="S39" s="12"/>
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
+      <c r="X39" s="12">
+        <v>4</v>
+      </c>
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
       <c r="AA39" s="12"/>
       <c r="AB39" s="12"/>
-      <c r="AC39" s="14">
-        <f t="shared" ref="AC39:AC53" si="7">SUM(E39:T39)</f>
-        <v>6.5</v>
-      </c>
+      <c r="AC39" s="14"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
+      <c r="B40" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -2290,126 +2266,54 @@
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
+      <c r="Y40" s="12">
+        <v>4</v>
+      </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="12"/>
       <c r="AB40" s="12"/>
-      <c r="AC40" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="15">
-        <f>SUM(E42:E43)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="15">
-        <f t="shared" ref="F41:T41" si="8">SUM(F42:F43)</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H41" s="15">
-        <f>SUM(H42:H43)</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="15">
-        <f>SUM(I42:I43)</f>
-        <v>0</v>
-      </c>
-      <c r="J41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O41" s="15">
-        <f>SUM(O42:O43)</f>
-        <v>0</v>
-      </c>
-      <c r="P41" s="15">
-        <f>SUM(P42:P43)</f>
-        <v>0</v>
-      </c>
-      <c r="Q41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T41" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U41" s="15">
-        <f t="shared" ref="U41:AB41" si="9">SUM(U42:U43)</f>
-        <v>0</v>
-      </c>
-      <c r="V41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="X41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Y41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB41" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AC41" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="22"/>
+      <c r="AC40" s="14"/>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B41" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="12"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="14"/>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B42" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -2430,19 +2334,20 @@
       <c r="V42" s="12"/>
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
-      <c r="Y42" s="12"/>
+      <c r="Y42" s="12">
+        <v>5</v>
+      </c>
       <c r="Z42" s="12"/>
       <c r="AA42" s="12"/>
       <c r="AB42" s="12"/>
-      <c r="AC42" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="AC42" s="14"/>
     </row>
     <row r="43" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="22"/>
+      <c r="B43" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
@@ -2463,126 +2368,54 @@
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
+      <c r="Y43" s="12">
+        <v>8</v>
+      </c>
       <c r="Z43" s="12"/>
       <c r="AA43" s="12"/>
       <c r="AB43" s="12"/>
-      <c r="AC43" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="15">
-        <f t="shared" ref="E44" si="10">SUM(E45:E47)</f>
-        <v>0</v>
-      </c>
-      <c r="F44" s="15">
-        <f>SUM(F45:F47)</f>
-        <v>0</v>
-      </c>
-      <c r="G44" s="15">
-        <f t="shared" ref="G44" si="11">SUM(G45:G47)</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="15">
-        <f>SUM(H45:H47)</f>
-        <v>0</v>
-      </c>
-      <c r="I44" s="15">
-        <f t="shared" ref="I44" si="12">SUM(I45:I47)</f>
-        <v>0</v>
-      </c>
-      <c r="J44" s="15">
-        <f t="shared" ref="J44:T44" si="13">SUM(J45:J47)</f>
-        <v>0</v>
-      </c>
-      <c r="K44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="O44" s="15">
-        <f>SUM(O45:O47)</f>
-        <v>0</v>
-      </c>
-      <c r="P44" s="15">
-        <f t="shared" ref="P44" si="14">SUM(P45:P47)</f>
-        <v>0</v>
-      </c>
-      <c r="Q44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="R44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="S44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="T44" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="U44" s="15">
-        <f t="shared" ref="U44:AB44" si="15">SUM(U45:U47)</f>
-        <v>0</v>
-      </c>
-      <c r="V44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="W44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="X44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="Y44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="Z44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AA44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AB44" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AC44" s="13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
+      <c r="AC43" s="14"/>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B44" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12">
+        <v>2</v>
+      </c>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="14"/>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B45" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -2604,18 +2437,19 @@
       <c r="W45" s="12"/>
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
-      <c r="Z45" s="12"/>
+      <c r="Z45" s="12">
+        <v>7</v>
+      </c>
       <c r="AA45" s="12"/>
       <c r="AB45" s="12"/>
-      <c r="AC45" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="20"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="22"/>
+      <c r="AC45" s="14"/>
+    </row>
+    <row r="46" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B46" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
@@ -2638,17 +2472,18 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
-      <c r="AA46" s="12"/>
+      <c r="AA46" s="12">
+        <v>5</v>
+      </c>
       <c r="AB46" s="12"/>
-      <c r="AC46" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="AC46" s="14"/>
     </row>
     <row r="47" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
+      <c r="B47" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -2671,126 +2506,52 @@
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
-      <c r="AA47" s="12"/>
+      <c r="AA47" s="12">
+        <v>4</v>
+      </c>
       <c r="AB47" s="12"/>
-      <c r="AC47" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="24" t="s">
+      <c r="AC47" s="14"/>
+    </row>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B48" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12"/>
+      <c r="V48" s="12"/>
+      <c r="W48" s="12"/>
+      <c r="X48" s="12"/>
+      <c r="Y48" s="12"/>
+      <c r="Z48" s="12"/>
+      <c r="AA48" s="12">
         <v>4</v>
       </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="15">
-        <f>SUM(E49:E51)</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="15">
-        <f>SUM(F49:F51)</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="15">
-        <f t="shared" ref="G48" si="16">SUM(G49:G51)</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="15">
-        <f>SUM(H49:H51)</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="15">
-        <f t="shared" ref="I48" si="17">SUM(I49:I51)</f>
-        <v>0</v>
-      </c>
-      <c r="J48" s="15">
-        <f t="shared" ref="J48:T48" si="18">SUM(J49:J51)</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="L48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O48" s="15">
-        <f>SUM(O49:O51)</f>
-        <v>0</v>
-      </c>
-      <c r="P48" s="15">
-        <f t="shared" ref="P48" si="19">SUM(P49:P51)</f>
-        <v>0</v>
-      </c>
-      <c r="Q48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="R48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="S48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="T48" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="U48" s="15">
-        <f t="shared" ref="U48:AB48" si="20">SUM(U49:U51)</f>
-        <v>0</v>
-      </c>
-      <c r="V48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="W48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="X48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="Y48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="Z48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AA48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AB48" s="15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AC48" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
+      <c r="AB48" s="12"/>
+      <c r="AC48" s="14"/>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B49" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -2813,19 +2574,18 @@
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
-      <c r="AA49" s="12"/>
+      <c r="AA49" s="12">
+        <v>3</v>
+      </c>
       <c r="AB49" s="12"/>
-      <c r="AC49" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
+      <c r="AC49" s="14"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B50" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="19"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -2849,18 +2609,17 @@
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
       <c r="AA50" s="12"/>
-      <c r="AB50" s="12"/>
-      <c r="AC50" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="AB50" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC50" s="14"/>
     </row>
     <row r="51" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B51" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
+      <c r="B51" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
@@ -2884,156 +2643,155 @@
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
       <c r="AA51" s="12"/>
-      <c r="AB51" s="12"/>
-      <c r="AC51" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="15">
-        <f>SUM(E53:E56)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="15">
-        <f>SUM(F53:F56)</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="15">
-        <f t="shared" ref="G52:T52" si="21">SUM(G53:G56)</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="15">
-        <f>SUM(H53:H55)</f>
-        <v>0</v>
-      </c>
-      <c r="I52" s="15">
-        <f t="shared" ref="I52" si="22">SUM(I53:I55)</f>
-        <v>0</v>
-      </c>
-      <c r="J52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="L52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="M52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="N52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="O52" s="15">
-        <f>SUM(O53:O55)</f>
-        <v>0</v>
-      </c>
-      <c r="P52" s="15">
-        <f t="shared" ref="P52" si="23">SUM(P53:P55)</f>
-        <v>0</v>
-      </c>
-      <c r="Q52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="R52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T52" s="15">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="U52" s="15">
-        <f t="shared" ref="U52:AB52" si="24">SUM(U53:U56)</f>
-        <v>0</v>
-      </c>
-      <c r="V52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="X52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Z52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="AA52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="AB52" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="AC52" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="12"/>
-      <c r="S53" s="12"/>
-      <c r="T53" s="12"/>
-      <c r="U53" s="12"/>
-      <c r="V53" s="12"/>
-      <c r="W53" s="12"/>
-      <c r="X53" s="12"/>
-      <c r="Y53" s="12"/>
-      <c r="Z53" s="12"/>
-      <c r="AA53" s="12"/>
-      <c r="AB53" s="12"/>
-      <c r="AC53" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
+      <c r="AB51" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC51" s="14"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="14">
+        <f>SUM(E52:T52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B53" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="34"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="15">
+        <f t="shared" ref="E53:T53" si="0">SUM(E54:E55)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L53" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N53" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q53" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S53" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="T53" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U53" s="15">
+        <f t="shared" ref="U53:AB53" si="1">SUM(U54:U55)</f>
+        <v>2</v>
+      </c>
+      <c r="V53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X53" s="15">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="Y53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z53" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC53" s="13">
+        <f>SUM(E53:AB53)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B54" s="26"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
@@ -3041,29 +2799,46 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
+      <c r="L54" s="12">
+        <v>3</v>
+      </c>
       <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
+      <c r="N54" s="12">
+        <v>1</v>
+      </c>
       <c r="O54" s="12"/>
       <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
+      <c r="Q54" s="12">
+        <v>1</v>
+      </c>
       <c r="R54" s="12"/>
-      <c r="S54" s="12"/>
+      <c r="S54" s="12">
+        <v>2.5</v>
+      </c>
       <c r="T54" s="12"/>
-      <c r="U54" s="12"/>
+      <c r="U54" s="12">
+        <v>2</v>
+      </c>
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
-      <c r="X54" s="12"/>
+      <c r="X54" s="12">
+        <v>1.5</v>
+      </c>
       <c r="Y54" s="12"/>
-      <c r="Z54" s="12"/>
+      <c r="Z54" s="12">
+        <v>1</v>
+      </c>
       <c r="AA54" s="12"/>
       <c r="AB54" s="12"/>
-      <c r="AC54" s="14"/>
-    </row>
-    <row r="55" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
+      <c r="AC54" s="14">
+        <f>SUM(E54:T54)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
@@ -3088,147 +2863,1000 @@
       <c r="Z55" s="12"/>
       <c r="AA55" s="12"/>
       <c r="AB55" s="12"/>
-      <c r="AC55" s="14"/>
-    </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
-      <c r="X56" s="12"/>
-      <c r="Y56" s="12"/>
-      <c r="Z56" s="12"/>
-      <c r="AA56" s="12"/>
-      <c r="AB56" s="12"/>
-      <c r="AC56" s="14">
+      <c r="AC55" s="14">
+        <f>SUM(E55:T55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="34"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="15">
+        <f>SUM(E57:E58)</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="15">
+        <f t="shared" ref="F56:T56" si="2">SUM(F57:F58)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H56" s="15">
+        <f>SUM(H57:H58)</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="15">
+        <f>SUM(I57:I58)</f>
+        <v>0</v>
+      </c>
+      <c r="J56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O56" s="15">
+        <f>SUM(O57:O58)</f>
+        <v>0</v>
+      </c>
+      <c r="P56" s="15">
+        <f>SUM(P57:P58)</f>
+        <v>0</v>
+      </c>
+      <c r="Q56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T56" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U56" s="15">
+        <f t="shared" ref="U56:AB56" si="3">SUM(U57:U58)</f>
+        <v>0</v>
+      </c>
+      <c r="V56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB56" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC56" s="13">
         <f>SUM(E56:T56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="13">
-        <f>SUM(E7,E41,E44,E48,E52)</f>
+    <row r="57" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="12"/>
+      <c r="V57" s="12"/>
+      <c r="W57" s="12"/>
+      <c r="X57" s="12"/>
+      <c r="Y57" s="12"/>
+      <c r="Z57" s="12"/>
+      <c r="AA57" s="12"/>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="14">
+        <f>SUM(E57:T57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="12"/>
+      <c r="V58" s="12"/>
+      <c r="W58" s="12"/>
+      <c r="X58" s="12"/>
+      <c r="Y58" s="12"/>
+      <c r="Z58" s="12"/>
+      <c r="AA58" s="12"/>
+      <c r="AB58" s="12"/>
+      <c r="AC58" s="14">
+        <f>SUM(E58:T58)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="15">
+        <f t="shared" ref="E59" si="4">SUM(E60:E62)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="15">
+        <f>SUM(F60:F62)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="15">
+        <f t="shared" ref="G59" si="5">SUM(G60:G62)</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="15">
+        <f>SUM(H60:H62)</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="15">
+        <f t="shared" ref="I59" si="6">SUM(I60:I62)</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="15">
+        <f t="shared" ref="J59:T59" si="7">SUM(J60:J62)</f>
+        <v>0</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O59" s="15">
+        <f>SUM(O60:O62)</f>
+        <v>0</v>
+      </c>
+      <c r="P59" s="15">
+        <f t="shared" ref="P59" si="8">SUM(P60:P62)</f>
+        <v>0</v>
+      </c>
+      <c r="Q59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T59" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U59" s="15">
+        <f t="shared" ref="U59:AB59" si="9">SUM(U60:U62)</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="X59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB59" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC59" s="13">
+        <f>SUM(E59:T59)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="12"/>
+      <c r="T60" s="12"/>
+      <c r="U60" s="12"/>
+      <c r="V60" s="12"/>
+      <c r="W60" s="12"/>
+      <c r="X60" s="12"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="14">
+        <f>SUM(E60:T60)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
+      <c r="R61" s="12"/>
+      <c r="S61" s="12"/>
+      <c r="T61" s="12"/>
+      <c r="U61" s="12"/>
+      <c r="V61" s="12"/>
+      <c r="W61" s="12"/>
+      <c r="X61" s="12"/>
+      <c r="Y61" s="12"/>
+      <c r="Z61" s="12"/>
+      <c r="AA61" s="12"/>
+      <c r="AB61" s="12"/>
+      <c r="AC61" s="14">
+        <f>SUM(E61:T61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
+      <c r="T62" s="12"/>
+      <c r="U62" s="12"/>
+      <c r="V62" s="12"/>
+      <c r="W62" s="12"/>
+      <c r="X62" s="12"/>
+      <c r="Y62" s="12"/>
+      <c r="Z62" s="12"/>
+      <c r="AA62" s="12"/>
+      <c r="AB62" s="12"/>
+      <c r="AC62" s="14">
+        <f>SUM(E62:T62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="15">
+        <f>SUM(E64:E66)</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="15">
+        <f>SUM(F64:F66)</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
+        <f t="shared" ref="G63" si="10">SUM(G64:G66)</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="15">
+        <f>SUM(H64:H66)</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="15">
+        <f t="shared" ref="I63" si="11">SUM(I64:I66)</f>
+        <v>0</v>
+      </c>
+      <c r="J63" s="15">
+        <f t="shared" ref="J63:T63" si="12">SUM(J64:J66)</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O63" s="15">
+        <f>SUM(O64:O66)</f>
+        <v>0</v>
+      </c>
+      <c r="P63" s="15">
+        <f t="shared" ref="P63" si="13">SUM(P64:P66)</f>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="T63" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U63" s="15">
+        <f t="shared" ref="U63:AB63" si="14">SUM(U64:U66)</f>
+        <v>0</v>
+      </c>
+      <c r="V63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Z63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB63" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AC63" s="14">
+        <f>SUM(E63:T63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="T64" s="12"/>
+      <c r="U64" s="12"/>
+      <c r="V64" s="12"/>
+      <c r="W64" s="12"/>
+      <c r="X64" s="12"/>
+      <c r="Y64" s="12"/>
+      <c r="Z64" s="12"/>
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="12"/>
+      <c r="AC64" s="14">
+        <f>SUM(E64:T64)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
+      <c r="R65" s="12"/>
+      <c r="S65" s="12"/>
+      <c r="T65" s="12"/>
+      <c r="U65" s="12"/>
+      <c r="V65" s="12"/>
+      <c r="W65" s="12"/>
+      <c r="X65" s="12"/>
+      <c r="Y65" s="12"/>
+      <c r="Z65" s="12"/>
+      <c r="AA65" s="12"/>
+      <c r="AB65" s="12"/>
+      <c r="AC65" s="14">
+        <f>SUM(E65:T65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B66" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="12"/>
+      <c r="S66" s="12"/>
+      <c r="T66" s="12"/>
+      <c r="U66" s="12"/>
+      <c r="V66" s="12"/>
+      <c r="W66" s="12"/>
+      <c r="X66" s="12"/>
+      <c r="Y66" s="12"/>
+      <c r="Z66" s="12"/>
+      <c r="AA66" s="12"/>
+      <c r="AB66" s="12"/>
+      <c r="AC66" s="14">
+        <f>SUM(E66:T66)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="13">
-        <f t="shared" ref="F57:T57" si="25">SUM(F7,F41,F44,F48,F52,F38)</f>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="15">
+        <f>SUM(E68:E71)</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="15">
+        <f>SUM(F68:F71)</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="15">
+        <f t="shared" ref="G67:T67" si="15">SUM(G68:G71)</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="15">
+        <f>SUM(H68:H70)</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="15">
+        <f t="shared" ref="I67" si="16">SUM(I68:I70)</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O67" s="15">
+        <f>SUM(O68:O70)</f>
+        <v>0</v>
+      </c>
+      <c r="P67" s="15">
+        <f t="shared" ref="P67" si="17">SUM(P68:P70)</f>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="R67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="T67" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U67" s="15">
+        <f t="shared" ref="U67:AB67" si="18">SUM(U68:U71)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="W67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Y67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Z67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB67" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC67" s="16">
+        <f>SUM(E67:T67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12"/>
+      <c r="Q68" s="12"/>
+      <c r="R68" s="12"/>
+      <c r="S68" s="12"/>
+      <c r="T68" s="12"/>
+      <c r="U68" s="12"/>
+      <c r="V68" s="12"/>
+      <c r="W68" s="12"/>
+      <c r="X68" s="12"/>
+      <c r="Y68" s="12"/>
+      <c r="Z68" s="12"/>
+      <c r="AA68" s="12"/>
+      <c r="AB68" s="12"/>
+      <c r="AC68" s="14">
+        <f>SUM(E68:T68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="12"/>
+      <c r="S69" s="12"/>
+      <c r="T69" s="12"/>
+      <c r="U69" s="12"/>
+      <c r="V69" s="12"/>
+      <c r="W69" s="12"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+      <c r="AA69" s="12"/>
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="14"/>
+    </row>
+    <row r="70" spans="2:29" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="R70" s="12"/>
+      <c r="S70" s="12"/>
+      <c r="T70" s="12"/>
+      <c r="U70" s="12"/>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="12"/>
+      <c r="AC70" s="14"/>
+    </row>
+    <row r="71" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12"/>
+      <c r="T71" s="12"/>
+      <c r="U71" s="12"/>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="12"/>
+      <c r="AC71" s="14">
+        <f>SUM(E71:T71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="13">
+        <f>SUM(E7,E56,E59,E63,E67)</f>
+        <v>8</v>
+      </c>
+      <c r="F72" s="13">
+        <f t="shared" ref="F72:T72" si="19">SUM(F7,F56,F59,F63,F67,F53)</f>
         <v>10</v>
       </c>
-      <c r="G57" s="13">
-        <f t="shared" si="25"/>
+      <c r="G72" s="13">
+        <f t="shared" si="19"/>
         <v>20</v>
       </c>
-      <c r="H57" s="13">
-        <f t="shared" si="25"/>
+      <c r="H72" s="13">
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="I57" s="13">
-        <f t="shared" si="25"/>
+      <c r="I72" s="13">
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="J57" s="13">
-        <f t="shared" si="25"/>
+      <c r="J72" s="13">
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
-      <c r="K57" s="13">
-        <f t="shared" si="25"/>
+      <c r="K72" s="13">
+        <f t="shared" si="19"/>
         <v>19</v>
       </c>
-      <c r="L57" s="13">
-        <f t="shared" si="25"/>
+      <c r="L72" s="13">
+        <f t="shared" si="19"/>
         <v>13</v>
       </c>
-      <c r="M57" s="13">
-        <f t="shared" si="25"/>
+      <c r="M72" s="13">
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
-      <c r="N57" s="13">
-        <f t="shared" si="25"/>
+      <c r="N72" s="13">
+        <f t="shared" si="19"/>
+        <v>13</v>
+      </c>
+      <c r="O72" s="13">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P72" s="13">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q72" s="13">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="R72" s="13">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="S72" s="13">
+        <f t="shared" si="19"/>
+        <v>12.5</v>
+      </c>
+      <c r="T72" s="13">
+        <f t="shared" si="19"/>
+        <v>13</v>
+      </c>
+      <c r="U72" s="13">
+        <f t="shared" ref="U72:AB72" si="20">SUM(U7,U56,U59,U63,U67,U53)</f>
         <v>12</v>
       </c>
-      <c r="O57" s="13">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="P57" s="13">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="Q57" s="13">
-        <f t="shared" si="25"/>
+      <c r="V72" s="13">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W72" s="13">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="X72" s="13">
+        <f t="shared" si="20"/>
+        <v>13.5</v>
+      </c>
+      <c r="Y72" s="13">
+        <f t="shared" si="20"/>
+        <v>18</v>
+      </c>
+      <c r="Z72" s="13">
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
-      <c r="R57" s="13">
-        <f t="shared" si="25"/>
+      <c r="AA72" s="13">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="AB72" s="13">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="AC72" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S57" s="13">
-        <f t="shared" si="25"/>
-        <v>12.5</v>
-      </c>
-      <c r="T57" s="13">
-        <f t="shared" si="25"/>
-        <v>13</v>
-      </c>
-      <c r="U57" s="13">
-        <f t="shared" ref="U57:AB57" si="26">SUM(U7,U41,U44,U48,U52,U38)</f>
-        <v>0</v>
-      </c>
-      <c r="V57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="W57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="X57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="Y57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="Z57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="AA57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="AB57" s="13">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="AC57" s="11" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="67">
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B33:D33"/>
@@ -3237,50 +3865,6 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>